<commit_message>
Political regions full fix
</commit_message>
<xml_diff>
--- a/GEP/Output_Clusters_Asigned_To_Countries/political_regions_37_af_1_df_wind.xlsx
+++ b/GEP/Output_Clusters_Asigned_To_Countries/political_regions_37_af_1_df_wind.xlsx
@@ -625,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.9999999999999986</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -733,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="AL2" t="n">
-        <v>0</v>
+        <v>0.9999999999999986</v>
       </c>
     </row>
     <row r="3">
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1.000000000000005</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="AL3" t="n">
-        <v>0</v>
+        <v>1.000000000000005</v>
       </c>
     </row>
     <row r="4">
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1.000000000000002</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -965,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="AL4" t="n">
-        <v>0</v>
+        <v>1.000000000000002</v>
       </c>
     </row>
     <row r="5">
@@ -982,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1081,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="AL5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.9999999999999971</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="AL6" t="n">
-        <v>0</v>
+        <v>0.9999999999999971</v>
       </c>
     </row>
     <row r="7">
@@ -1220,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1313,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="AL7" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -1339,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.999999999999987</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="AL8" t="n">
-        <v>0</v>
+        <v>0.999999999999987</v>
       </c>
     </row>
     <row r="9">
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.9999999999999961</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -1545,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="AL9" t="n">
-        <v>0</v>
+        <v>0.9999999999999961</v>
       </c>
     </row>
     <row r="10">
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.9999999999999979</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="AL10" t="n">
-        <v>0</v>
+        <v>0.9999999999999979</v>
       </c>
     </row>
     <row r="11">
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="AL11" t="n">
-        <v>0</v>
+        <v>0.9999999999999996</v>
       </c>
     </row>
     <row r="12">
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -1893,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="AL12" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -1934,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="AL13" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -2053,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>0.9999999999999993</v>
       </c>
       <c r="O14" t="n">
         <v>0</v>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="AL14" t="n">
-        <v>0</v>
+        <v>0.9999999999999993</v>
       </c>
     </row>
     <row r="15">
@@ -2291,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>0.9999999999999902</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="AL16" t="n">
-        <v>0</v>
+        <v>0.9999999999999902</v>
       </c>
     </row>
     <row r="17">
@@ -2410,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="AL17" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -2529,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -2589,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="AL18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>0</v>
+        <v>0.9999999999999991</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="AL19" t="n">
-        <v>0</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="20">
@@ -2767,7 +2767,7 @@
         <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>0</v>
+        <v>0.9999999999999926</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -2821,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="AL20" t="n">
-        <v>0</v>
+        <v>0.9999999999999926</v>
       </c>
     </row>
     <row r="21">
@@ -2886,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" t="n">
         <v>0</v>
@@ -2937,7 +2937,7 @@
         <v>0</v>
       </c>
       <c r="AL21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>0</v>
+        <v>0.9999999999999877</v>
       </c>
       <c r="X23" t="n">
         <v>0</v>
@@ -3169,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="AL23" t="n">
-        <v>0</v>
+        <v>0.9999999999999877</v>
       </c>
     </row>
     <row r="24">
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y24" t="n">
         <v>0</v>
@@ -3285,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="AL24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -3362,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="Y25" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="Z25" t="n">
         <v>0</v>
@@ -3401,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="AL25" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
     </row>
     <row r="26">
@@ -3481,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="Z26" t="n">
-        <v>0</v>
+        <v>0.9999999999999989</v>
       </c>
       <c r="AA26" t="n">
         <v>0</v>
@@ -3517,7 +3517,7 @@
         <v>0</v>
       </c>
       <c r="AL26" t="n">
-        <v>0</v>
+        <v>0.9999999999999989</v>
       </c>
     </row>
     <row r="27">
@@ -3600,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="AA27" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="AB27" t="n">
         <v>0</v>
@@ -3633,7 +3633,7 @@
         <v>0</v>
       </c>
       <c r="AL27" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
     </row>
     <row r="28">
@@ -3719,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="AB28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC28" t="n">
         <v>0</v>
@@ -3749,7 +3749,7 @@
         <v>0</v>
       </c>
       <c r="AL28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -3838,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="AC29" t="n">
-        <v>0</v>
+        <v>1.000000000000002</v>
       </c>
       <c r="AD29" t="n">
         <v>0</v>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="AL29" t="n">
-        <v>0</v>
+        <v>1.000000000000002</v>
       </c>
     </row>
     <row r="30">
@@ -3957,7 +3957,7 @@
         <v>0</v>
       </c>
       <c r="AD30" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="AE30" t="n">
         <v>0</v>
@@ -3972,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="AI30" t="n">
-        <v>0</v>
+        <v>0.008849557522123894</v>
       </c>
       <c r="AJ30" t="n">
         <v>0</v>
@@ -3981,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="AL30" t="n">
-        <v>0</v>
+        <v>1.008849557522125</v>
       </c>
     </row>
     <row r="31">
@@ -4076,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>0</v>
+        <v>1.000000000000011</v>
       </c>
       <c r="AF31" t="n">
         <v>0</v>
@@ -4097,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="AL31" t="n">
-        <v>0</v>
+        <v>1.000000000000011</v>
       </c>
     </row>
     <row r="32">
@@ -4195,7 +4195,7 @@
         <v>0</v>
       </c>
       <c r="AF32" t="n">
-        <v>0</v>
+        <v>0.9999999999999942</v>
       </c>
       <c r="AG32" t="n">
         <v>0</v>
@@ -4213,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="AL32" t="n">
-        <v>0</v>
+        <v>0.9999999999999942</v>
       </c>
     </row>
     <row r="33">
@@ -4314,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="AG33" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="AH33" t="n">
         <v>0</v>
@@ -4329,7 +4329,7 @@
         <v>0</v>
       </c>
       <c r="AL33" t="n">
-        <v>0</v>
+        <v>1.000000000000001</v>
       </c>
     </row>
     <row r="34">
@@ -4433,7 +4433,7 @@
         <v>0</v>
       </c>
       <c r="AH34" t="n">
-        <v>0</v>
+        <v>0.9999999999999992</v>
       </c>
       <c r="AI34" t="n">
         <v>0</v>
@@ -4445,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="AL34" t="n">
-        <v>0</v>
+        <v>0.9999999999999992</v>
       </c>
     </row>
     <row r="35">
@@ -4552,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="AI35" t="n">
-        <v>0</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="AJ35" t="n">
         <v>0</v>
@@ -4561,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="AL35" t="n">
-        <v>0</v>
+        <v>0.9999999999999996</v>
       </c>
     </row>
     <row r="36">
@@ -4671,13 +4671,13 @@
         <v>0</v>
       </c>
       <c r="AJ36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK36" t="n">
         <v>0</v>
       </c>
       <c r="AL36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -4790,10 +4790,10 @@
         <v>0</v>
       </c>
       <c r="AK37" t="n">
-        <v>0</v>
+        <v>1.000000000000022</v>
       </c>
       <c r="AL37" t="n">
-        <v>0</v>
+        <v>1.000000000000022</v>
       </c>
     </row>
     <row r="38">

</xml_diff>